<commit_message>
Implement FineTunedModel for integrating end-to-end
</commit_message>
<xml_diff>
--- a/evaluation/v2/evalute-integration.xlsx
+++ b/evaluation/v2/evalute-integration.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="421">
   <si>
     <t>Everyday Cheek Liptint</t>
   </si>
@@ -295,6 +295,12 @@
     <t>Kelopak Mata</t>
   </si>
   <si>
+    <t>3.3</t>
+  </si>
+  <si>
+    <t>gr</t>
+  </si>
+  <si>
     <t>Acnederm Face Powder</t>
   </si>
   <si>
@@ -316,6 +322,12 @@
     <t>Pipi</t>
   </si>
   <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
     <t>Exclusive Liquid Foundation</t>
   </si>
   <si>
@@ -337,6 +349,12 @@
     <t>20 ml</t>
   </si>
   <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>ml</t>
+  </si>
+  <si>
     <t>Exclusive Two Way Cake</t>
   </si>
   <si>
@@ -451,699 +469,708 @@
     <t>13 Beige</t>
   </si>
   <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Instaperfect Spotlight Chromatic Eye Palette</t>
+  </si>
+  <si>
+    <t>10 g</t>
+  </si>
+  <si>
+    <t>Instaperfect Geniustwist Matic Contour Brow Brushed</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>Deep Grey</t>
+  </si>
+  <si>
+    <t>02 Deep</t>
+  </si>
+  <si>
+    <t>Alis</t>
+  </si>
+  <si>
+    <t>0.25 g</t>
+  </si>
+  <si>
+    <t>Instaperfect Hypergetic Precise Black Liner</t>
+  </si>
+  <si>
+    <t>Instaperfect Mattesetter Lip Matte Paint</t>
+  </si>
+  <si>
+    <t>01 Glee</t>
+  </si>
+  <si>
+    <t>05 Hype</t>
+  </si>
+  <si>
+    <t>5.5</t>
+  </si>
+  <si>
+    <t>Instaperfect Quick Fix Cover Correct Concealer</t>
+  </si>
+  <si>
+    <t>1.8</t>
+  </si>
+  <si>
+    <t>Instaperfect Dynamatic Microsmooth Liner</t>
+  </si>
+  <si>
+    <t>0.2 g</t>
+  </si>
+  <si>
+    <t>Refill Instaperfect Mineralight Matte Bb Cushion</t>
+  </si>
+  <si>
+    <t>11 Fair</t>
+  </si>
+  <si>
+    <t>14 Créme</t>
+  </si>
+  <si>
+    <t>Instaperfect Gloss Chic Lip Crayon</t>
+  </si>
+  <si>
+    <t>01 Rhythm</t>
+  </si>
+  <si>
+    <t>02 Clue</t>
+  </si>
+  <si>
+    <t>03 Mind</t>
+  </si>
+  <si>
+    <t>2.7 g</t>
+  </si>
+  <si>
+    <t>2.7</t>
+  </si>
+  <si>
+    <t>Instaperfect Mattetitude Matte Stain Lipstick</t>
+  </si>
+  <si>
+    <t>03 Femme</t>
+  </si>
+  <si>
+    <t>04 Buzz</t>
+  </si>
+  <si>
+    <t>01 Swing</t>
+  </si>
+  <si>
+    <t>05 Flux</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>Instaperfect Mattecentric Lip Crayon</t>
+  </si>
+  <si>
+    <t>05 Sense</t>
+  </si>
+  <si>
+    <t>06 Soul</t>
+  </si>
+  <si>
+    <t>04 Joy</t>
+  </si>
+  <si>
+    <t>03 Honor</t>
+  </si>
+  <si>
+    <t>02 Morale</t>
+  </si>
+  <si>
+    <t>01 Pace</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Instaperfect Matte Fit Powder Foundation</t>
+  </si>
+  <si>
+    <t>14 Crème</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Refill Instaperfect Matte Fit Powder Foundation</t>
+  </si>
+  <si>
+    <t>14 Creme</t>
+  </si>
+  <si>
+    <t>Colorfit Velvet Matte Lip Mousse</t>
+  </si>
+  <si>
+    <t>08 Brown Creator</t>
+  </si>
+  <si>
+    <t>01 Brown Dreamer</t>
+  </si>
+  <si>
+    <t>05 Artisan Mauve</t>
+  </si>
+  <si>
+    <t>04 Pink Sweetheart</t>
+  </si>
+  <si>
+    <t>02 Joyful Orange</t>
+  </si>
+  <si>
+    <t>03 Rose Ballerina</t>
+  </si>
+  <si>
+    <t>07 Red Pioneer</t>
+  </si>
+  <si>
+    <t>06 Fuchsia Lover</t>
+  </si>
+  <si>
+    <t>Magic Potion</t>
+  </si>
+  <si>
+    <t>Emina</t>
+  </si>
+  <si>
+    <t>01 Scarlett</t>
+  </si>
+  <si>
+    <t>02 Sunglow</t>
+  </si>
+  <si>
+    <t>03 Smitten</t>
+  </si>
+  <si>
+    <t>04 Sienna</t>
+  </si>
+  <si>
+    <t>05 Summer</t>
+  </si>
+  <si>
+    <t>06 Sassy</t>
+  </si>
+  <si>
+    <t>5.5 ml</t>
+  </si>
+  <si>
+    <t>Glossy Stain</t>
+  </si>
+  <si>
+    <t>02 Apple Shower</t>
+  </si>
+  <si>
+    <t>05 Spring Dazzle</t>
+  </si>
+  <si>
+    <t>03 Candy Rain</t>
+  </si>
+  <si>
+    <t>Cheek Lit Pressed Blush</t>
+  </si>
+  <si>
+    <t>Peach</t>
+  </si>
+  <si>
+    <t>Pink</t>
+  </si>
+  <si>
+    <t>Bittersweet</t>
+  </si>
+  <si>
+    <t>Cherry Blossoms</t>
+  </si>
+  <si>
+    <t>Cotton Candy</t>
+  </si>
+  <si>
+    <t>Marshmallow Lady</t>
+  </si>
+  <si>
+    <t>Sugarcane</t>
+  </si>
+  <si>
+    <t>Violet Berry</t>
+  </si>
+  <si>
+    <t>Cheek Lit Cream Blush</t>
+  </si>
+  <si>
+    <t>Nudie Brown</t>
+  </si>
+  <si>
+    <t>Violet</t>
+  </si>
+  <si>
+    <t>Beauty Bliss Bb Cream</t>
+  </si>
+  <si>
+    <t>Light</t>
+  </si>
+  <si>
+    <t>Caaramel</t>
+  </si>
+  <si>
+    <t>Caramel</t>
+  </si>
+  <si>
+    <t>Natural</t>
+  </si>
+  <si>
+    <t>Bare With Me Mineral Cushion</t>
+  </si>
+  <si>
+    <t>Bright Stuff Loose Powder</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>Pore Ranger</t>
+  </si>
+  <si>
+    <t>Daily Matte Loose Powder</t>
+  </si>
+  <si>
+    <t>Powder</t>
+  </si>
+  <si>
+    <t>Pop Rouge Pressed Eye Shadow</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Colorful</t>
+  </si>
+  <si>
+    <t>Gelato</t>
+  </si>
+  <si>
+    <t>Nude</t>
+  </si>
+  <si>
+    <t>Purple</t>
+  </si>
+  <si>
+    <t>Romantic</t>
+  </si>
+  <si>
+    <t>Posh</t>
+  </si>
+  <si>
+    <t>Brick</t>
+  </si>
+  <si>
+    <t>Frosted</t>
+  </si>
+  <si>
+    <t>City Chic Cc Cake</t>
+  </si>
+  <si>
+    <t>Latte</t>
+  </si>
+  <si>
+    <t>Butterscotch</t>
+  </si>
+  <si>
+    <t>Meringue</t>
+  </si>
+  <si>
+    <t>Star Lash Aqua Mascara</t>
+  </si>
+  <si>
+    <t>5 g</t>
+  </si>
+  <si>
+    <t>Agent Of Brow</t>
+  </si>
+  <si>
+    <t>1.2 g</t>
+  </si>
+  <si>
+    <t>Eye Do Crayon Pour Les Yeux</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Deep Purple</t>
+  </si>
+  <si>
+    <t>0.20</t>
+  </si>
+  <si>
+    <t>Top Secret Eyebrow</t>
+  </si>
+  <si>
+    <t>2.9 g</t>
+  </si>
+  <si>
+    <t>Double Agent Eyebrow</t>
+  </si>
+  <si>
+    <t>Creamatte Metallic Edition</t>
+  </si>
+  <si>
+    <t>01 Berry Stardust</t>
+  </si>
+  <si>
+    <t>02 Sunset Sparks</t>
+  </si>
+  <si>
+    <t>03 Unicorn Glow</t>
+  </si>
+  <si>
+    <t>5.5 g</t>
+  </si>
+  <si>
+    <t>Soulmatte Lipstick</t>
+  </si>
+  <si>
+    <t>01 Enchantress</t>
+  </si>
+  <si>
+    <t>02 Unicorn</t>
+  </si>
+  <si>
+    <t>03 Fairy Fantasy</t>
+  </si>
+  <si>
+    <t>04 Love Spell</t>
+  </si>
+  <si>
+    <t>05 Feathers</t>
+  </si>
+  <si>
+    <t>06 Red Queen</t>
+  </si>
+  <si>
+    <t>Sugar Rush Lipstick</t>
+  </si>
+  <si>
+    <t>01 Pink Velvet</t>
+  </si>
+  <si>
+    <t>02 Cookie Dough</t>
+  </si>
+  <si>
+    <t>03 Cherry Bomb</t>
+  </si>
+  <si>
+    <t>04 Maroon Macaroon</t>
+  </si>
+  <si>
+    <t>Creamytint</t>
+  </si>
+  <si>
+    <t>Creamatte</t>
+  </si>
+  <si>
+    <t>01 Chocolava</t>
+  </si>
+  <si>
+    <t>02 Fuzzy Wuzzy</t>
+  </si>
+  <si>
+    <t>04 Frostbite</t>
+  </si>
+  <si>
+    <t>05 Flamingo</t>
+  </si>
+  <si>
+    <t>06 Jelly Bean</t>
+  </si>
+  <si>
+    <t>07 Tumbleweed</t>
+  </si>
+  <si>
+    <t>08 Pumpkin Spice</t>
+  </si>
+  <si>
+    <t>09 Baby Fox</t>
+  </si>
+  <si>
+    <t>10 Starfish</t>
+  </si>
+  <si>
+    <t>11 Amazeballs</t>
+  </si>
+  <si>
+    <t>12 Perky Plum</t>
+  </si>
+  <si>
+    <t>13 Beet Bites</t>
+  </si>
+  <si>
+    <t>14 Gingerale</t>
+  </si>
+  <si>
+    <t>15 Chocopuff</t>
+  </si>
+  <si>
+    <t>Lip Cushion</t>
+  </si>
+  <si>
+    <t>Tinted Lipbalm</t>
+  </si>
+  <si>
+    <t>Liquid Lip Shine</t>
+  </si>
+  <si>
+    <t>Buttery Nude</t>
+  </si>
+  <si>
+    <t>Carnation Pink</t>
+  </si>
+  <si>
+    <t>Cerise Red</t>
+  </si>
+  <si>
+    <t>Wineberry</t>
+  </si>
+  <si>
+    <t>4.5 ml</t>
+  </si>
+  <si>
+    <t>Smoochies Lipbalm</t>
+  </si>
+  <si>
+    <t>Cucumber Juice</t>
+  </si>
+  <si>
+    <t>Lemonade</t>
+  </si>
+  <si>
+    <t>3.7 g</t>
+  </si>
+  <si>
+    <t>Lipstick</t>
+  </si>
+  <si>
+    <t>Sariayu</t>
+  </si>
+  <si>
+    <t>Nias 02</t>
+  </si>
+  <si>
+    <t>Alun Serunai 01</t>
+  </si>
+  <si>
+    <t>Borneo 01</t>
+  </si>
+  <si>
+    <t>Petikan Sitar 01</t>
+  </si>
+  <si>
+    <t>Petikan Sitar 02</t>
+  </si>
+  <si>
+    <t>Borneo 03</t>
+  </si>
+  <si>
+    <t>Borneo 02</t>
+  </si>
+  <si>
+    <t>Toba 02</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Marunda 3</t>
+  </si>
+  <si>
+    <t>Marunda 2</t>
+  </si>
+  <si>
+    <t>Color Trend 2019 Hydra Lip Tint</t>
+  </si>
+  <si>
+    <t>Wi 03</t>
+  </si>
+  <si>
+    <t>Color Trend 2019 Lite Lip Cream</t>
+  </si>
+  <si>
+    <t>Wi 04</t>
+  </si>
+  <si>
+    <t>Wi 01</t>
+  </si>
+  <si>
+    <t>Wi 02</t>
+  </si>
+  <si>
+    <t>Lip Care</t>
+  </si>
+  <si>
+    <t>Color Trend 2016 Duo Lip Color</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>Color Trend 2017 Duo Lip Color</t>
+  </si>
+  <si>
+    <t>Gl 01</t>
+  </si>
+  <si>
+    <t>Gl 06</t>
+  </si>
+  <si>
+    <t>Gl 05</t>
+  </si>
+  <si>
+    <t>Color Trend 2018 Lip Cream</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>Color Trend 2018 Lip Metallic</t>
+  </si>
+  <si>
+    <t>Lip Colour Matte</t>
+  </si>
+  <si>
+    <t>Lip Color Matte</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Ct 19 Lite Lip Cream</t>
+  </si>
+  <si>
+    <t>Wi</t>
+  </si>
+  <si>
+    <t>Trend 2017 Duo Lip Color</t>
+  </si>
+  <si>
+    <t>Gl 03</t>
+  </si>
+  <si>
+    <t>Two Way Cake</t>
+  </si>
+  <si>
+    <t>Dark</t>
+  </si>
+  <si>
+    <t>03 Dark</t>
+  </si>
+  <si>
+    <t>02 Natural</t>
+  </si>
+  <si>
+    <t>Moisturizer</t>
+  </si>
+  <si>
+    <t>Jeruk</t>
+  </si>
+  <si>
+    <t>Leher</t>
+  </si>
+  <si>
+    <t>Color Trend 2020 Lip Cheek</t>
+  </si>
+  <si>
+    <t>S 03</t>
+  </si>
+  <si>
+    <t>Serene</t>
+  </si>
+  <si>
+    <t>S 02</t>
+  </si>
+  <si>
+    <t>Freshly</t>
+  </si>
+  <si>
+    <t>S 01</t>
+  </si>
+  <si>
+    <t>Rosy</t>
+  </si>
+  <si>
+    <t>35 gr</t>
+  </si>
+  <si>
+    <t>Two Way Cake Energizing Aromatic Refill</t>
+  </si>
+  <si>
+    <t>Putih Langsat</t>
+  </si>
+  <si>
+    <t>Alas Bedak Energizing Aromatic</t>
+  </si>
+  <si>
+    <t>Kuning Gading</t>
+  </si>
+  <si>
+    <t>Kuning Langsat</t>
+  </si>
+  <si>
+    <t>Kuning Pengantin</t>
+  </si>
+  <si>
+    <t>Sawo Matang</t>
+  </si>
+  <si>
+    <t>Color Trend 2020 Cheek Palette</t>
+  </si>
+  <si>
+    <t>Pinkish</t>
+  </si>
+  <si>
+    <t>Loose Powder</t>
+  </si>
+  <si>
+    <t>Butiran</t>
+  </si>
+  <si>
+    <t>Creamy Foundation</t>
+  </si>
+  <si>
     <t>15 g</t>
   </si>
   <si>
-    <t>Instaperfect Spotlight Chromatic Eye Palette</t>
-  </si>
-  <si>
-    <t>10 g</t>
-  </si>
-  <si>
-    <t>Instaperfect Geniustwist Matic Contour Brow Brushed</t>
-  </si>
-  <si>
-    <t>01 Brown</t>
-  </si>
-  <si>
-    <t>Deep Grey</t>
-  </si>
-  <si>
-    <t>02 Deep Grey</t>
-  </si>
-  <si>
-    <t>Brown</t>
-  </si>
-  <si>
-    <t>Alis</t>
-  </si>
-  <si>
-    <t>0.25 g</t>
-  </si>
-  <si>
-    <t>Instaperfect Hypergetic Precise Black Liner</t>
-  </si>
-  <si>
-    <t>Instaperfect Mattesetter Lip Matte Paint</t>
-  </si>
-  <si>
-    <t>01 Glee</t>
-  </si>
-  <si>
-    <t>05 Hype</t>
-  </si>
-  <si>
-    <t>5.5 g</t>
-  </si>
-  <si>
-    <t>Instaperfect Quick Fix Cover Correct Concealer</t>
-  </si>
-  <si>
-    <t>1.8 g</t>
-  </si>
-  <si>
-    <t>Instaperfect Dynamatic Microsmooth Liner</t>
-  </si>
-  <si>
-    <t>0.2 g</t>
-  </si>
-  <si>
-    <t>Refill Instaperfect Mineralight Matte Bb Cushion</t>
-  </si>
-  <si>
-    <t>11 Fair</t>
-  </si>
-  <si>
-    <t>14 Créme</t>
-  </si>
-  <si>
-    <t>Instaperfect Gloss Chic Lip Crayon</t>
-  </si>
-  <si>
-    <t>01 Rhythm</t>
-  </si>
-  <si>
-    <t>02 Clue</t>
-  </si>
-  <si>
-    <t>03 Mind</t>
-  </si>
-  <si>
-    <t>2.7 g</t>
-  </si>
-  <si>
-    <t>Instaperfect Mattetitude Matte Stain Lipstick</t>
-  </si>
-  <si>
-    <t>03 Femme</t>
-  </si>
-  <si>
-    <t>04 Buzz</t>
-  </si>
-  <si>
-    <t>01 Swing</t>
-  </si>
-  <si>
-    <t>05 Flux</t>
-  </si>
-  <si>
-    <t>Instaperfect Mattecentric Lip Crayon</t>
-  </si>
-  <si>
-    <t>05 Sense</t>
-  </si>
-  <si>
-    <t>06 Soul</t>
-  </si>
-  <si>
-    <t>04 Joy</t>
-  </si>
-  <si>
-    <t>03 Honor</t>
-  </si>
-  <si>
-    <t>02 Morale</t>
-  </si>
-  <si>
-    <t>01 Pace</t>
-  </si>
-  <si>
-    <t>3 g</t>
-  </si>
-  <si>
-    <t>Instaperfect Matte Fit Powder Foundation</t>
-  </si>
-  <si>
-    <t>14 Crème</t>
-  </si>
-  <si>
-    <t>13 g</t>
-  </si>
-  <si>
-    <t>Refill Instaperfect Matte Fit Powder Foundation</t>
-  </si>
-  <si>
-    <t>14 Creme</t>
-  </si>
-  <si>
-    <t>Colorfit Velvet Matte Lip Mousse</t>
-  </si>
-  <si>
-    <t>08 Brown Creator</t>
-  </si>
-  <si>
-    <t>01 Brown Dreamer</t>
-  </si>
-  <si>
-    <t>05 Artisan Mauve</t>
-  </si>
-  <si>
-    <t>04 Pink Sweetheart</t>
-  </si>
-  <si>
-    <t>02 Joyful Orange</t>
-  </si>
-  <si>
-    <t>03 Rose Ballerina</t>
-  </si>
-  <si>
-    <t>07 Red Pioneer</t>
-  </si>
-  <si>
-    <t>06 Fuchsia Lover</t>
-  </si>
-  <si>
-    <t>Magic Potion</t>
-  </si>
-  <si>
-    <t>Emina</t>
-  </si>
-  <si>
-    <t>01 Scarlett</t>
-  </si>
-  <si>
-    <t>02 Sunglow</t>
-  </si>
-  <si>
-    <t>03 Smitten</t>
-  </si>
-  <si>
-    <t>04 Sienna</t>
-  </si>
-  <si>
-    <t>05 Summer</t>
-  </si>
-  <si>
-    <t>06 Sassy</t>
-  </si>
-  <si>
-    <t>5.5 ml</t>
-  </si>
-  <si>
-    <t>Glossy Stain</t>
-  </si>
-  <si>
-    <t>02 Apple Shower</t>
-  </si>
-  <si>
-    <t>05 Spring Dazzle</t>
-  </si>
-  <si>
-    <t>03 Candy Rain</t>
-  </si>
-  <si>
-    <t>Cheek Lit Pressed Blush</t>
-  </si>
-  <si>
-    <t>Peach</t>
-  </si>
-  <si>
-    <t>Pink</t>
-  </si>
-  <si>
-    <t>Bittersweet</t>
-  </si>
-  <si>
-    <t>Cherry Blossoms</t>
-  </si>
-  <si>
-    <t>Cotton Candy</t>
-  </si>
-  <si>
-    <t>Marshmallow Lady</t>
-  </si>
-  <si>
-    <t>Sugarcane</t>
-  </si>
-  <si>
-    <t>Violet Berry</t>
-  </si>
-  <si>
-    <t>Cheek Lit Cream Blush</t>
-  </si>
-  <si>
-    <t>Nudie Brown</t>
-  </si>
-  <si>
-    <t>Violet</t>
-  </si>
-  <si>
-    <t>Beauty Bliss Bb Cream</t>
-  </si>
-  <si>
-    <t>Light</t>
-  </si>
-  <si>
-    <t>Caaramel</t>
-  </si>
-  <si>
-    <t>Caramel</t>
-  </si>
-  <si>
-    <t>Natural</t>
-  </si>
-  <si>
-    <t>Bare With Me Mineral Cushion</t>
-  </si>
-  <si>
-    <t>Bright Stuff Loose Powder</t>
-  </si>
-  <si>
-    <t>55 g</t>
-  </si>
-  <si>
-    <t>Pore Ranger</t>
-  </si>
-  <si>
-    <t>Daily Matte Loose Powder</t>
-  </si>
-  <si>
-    <t>Powder</t>
-  </si>
-  <si>
-    <t>Pop Rouge Pressed Eye Shadow</t>
-  </si>
-  <si>
-    <t>Blue</t>
-  </si>
-  <si>
-    <t>Colorful</t>
-  </si>
-  <si>
-    <t>Gelato</t>
-  </si>
-  <si>
-    <t>Nude</t>
-  </si>
-  <si>
-    <t>Purple</t>
-  </si>
-  <si>
-    <t>Romantic</t>
-  </si>
-  <si>
-    <t>Posh</t>
-  </si>
-  <si>
-    <t>Brick</t>
-  </si>
-  <si>
-    <t>Frosted</t>
-  </si>
-  <si>
-    <t>City Chic Cc Cake</t>
-  </si>
-  <si>
-    <t>Latte</t>
-  </si>
-  <si>
-    <t>Butterscotch</t>
-  </si>
-  <si>
-    <t>Meringue</t>
-  </si>
-  <si>
-    <t>Star Lash Aqua Mascara</t>
-  </si>
-  <si>
-    <t>5 g</t>
-  </si>
-  <si>
-    <t>Agent Of Brow</t>
-  </si>
-  <si>
-    <t>1.2 g</t>
-  </si>
-  <si>
-    <t>Eye Do Crayon Pour Les Yeux</t>
-  </si>
-  <si>
-    <t>Black</t>
-  </si>
-  <si>
-    <t>Deep Purple</t>
-  </si>
-  <si>
-    <t>0.20 g</t>
-  </si>
-  <si>
-    <t>Top Secret Eyebrow</t>
-  </si>
-  <si>
-    <t>2.9 g</t>
-  </si>
-  <si>
-    <t>Double Agent Eyebrow</t>
-  </si>
-  <si>
-    <t>Creamatte Metallic Edition</t>
-  </si>
-  <si>
-    <t>01 Berry Stardust</t>
-  </si>
-  <si>
-    <t>02 Sunset Sparks</t>
-  </si>
-  <si>
-    <t>03 Unicorn Glow</t>
-  </si>
-  <si>
-    <t>Soulmatte Lipstick</t>
-  </si>
-  <si>
-    <t>01 Enchantress</t>
-  </si>
-  <si>
-    <t>02 Unicorn</t>
-  </si>
-  <si>
-    <t>03 Fairy Fantasy</t>
-  </si>
-  <si>
-    <t>04 Love Spell</t>
-  </si>
-  <si>
-    <t>05 Feathers</t>
-  </si>
-  <si>
-    <t>06 Red Queen</t>
-  </si>
-  <si>
-    <t>Sugar Rush Lipstick</t>
-  </si>
-  <si>
-    <t>01 Pink Velvet</t>
-  </si>
-  <si>
-    <t>02 Cookie Dough</t>
-  </si>
-  <si>
-    <t>03 Cherry Bomb</t>
-  </si>
-  <si>
-    <t>04 Maroon Macaroon</t>
-  </si>
-  <si>
-    <t>Creamytint</t>
-  </si>
-  <si>
-    <t>Creamatte</t>
-  </si>
-  <si>
-    <t>01 Chocolava</t>
-  </si>
-  <si>
-    <t>02 Fuzzy Wuzzy</t>
-  </si>
-  <si>
-    <t>04 Frostbite</t>
-  </si>
-  <si>
-    <t>05 Flamingo</t>
-  </si>
-  <si>
-    <t>06 Jelly Bean</t>
-  </si>
-  <si>
-    <t>07 Tumbleweed</t>
-  </si>
-  <si>
-    <t>08 Pumpkin Spice</t>
-  </si>
-  <si>
-    <t>09 Baby Fox</t>
-  </si>
-  <si>
-    <t>10 Starfish</t>
-  </si>
-  <si>
-    <t>11 Amazeballs</t>
-  </si>
-  <si>
-    <t>12 Perky Plum</t>
-  </si>
-  <si>
-    <t>13 Beet Bites</t>
-  </si>
-  <si>
-    <t>14 Gingerale</t>
-  </si>
-  <si>
-    <t>15 Chocopuff</t>
-  </si>
-  <si>
-    <t>Lip Cushion</t>
-  </si>
-  <si>
-    <t>Tinted Lipbalm</t>
-  </si>
-  <si>
-    <t>Liquid Lip Shine</t>
-  </si>
-  <si>
-    <t>Buttery Nude</t>
-  </si>
-  <si>
-    <t>Carnation Pink</t>
-  </si>
-  <si>
-    <t>Cerise Red</t>
-  </si>
-  <si>
-    <t>Wineberry</t>
-  </si>
-  <si>
-    <t>4.5 ml</t>
-  </si>
-  <si>
-    <t>Smoochies Lipbalm</t>
-  </si>
-  <si>
-    <t>Cucumber Juice</t>
-  </si>
-  <si>
-    <t>Lemonade</t>
-  </si>
-  <si>
-    <t>3.7 g</t>
-  </si>
-  <si>
-    <t>Lipstick</t>
-  </si>
-  <si>
-    <t>Sariayu</t>
-  </si>
-  <si>
-    <t>Nias 02</t>
-  </si>
-  <si>
-    <t>Alun Serunai 01</t>
-  </si>
-  <si>
-    <t>Borneo 01</t>
-  </si>
-  <si>
-    <t>Petikan Sitar 01</t>
-  </si>
-  <si>
-    <t>Petikan Sitar 02</t>
-  </si>
-  <si>
-    <t>Borneo 03</t>
-  </si>
-  <si>
-    <t>Borneo 02</t>
-  </si>
-  <si>
-    <t>Toba 02</t>
-  </si>
-  <si>
-    <t>No 5</t>
-  </si>
-  <si>
-    <t>Marunda 3</t>
-  </si>
-  <si>
-    <t>Marunda 2</t>
-  </si>
-  <si>
-    <t>Color Trend 2019 Hydra Lip Tint</t>
-  </si>
-  <si>
-    <t>Wi 03</t>
-  </si>
-  <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>Color Trend 2019 Lite Lip Cream</t>
-  </si>
-  <si>
-    <t>Wi 04</t>
-  </si>
-  <si>
-    <t>Wi 01</t>
-  </si>
-  <si>
-    <t>Wi 02</t>
-  </si>
-  <si>
-    <t>Lip Care</t>
-  </si>
-  <si>
-    <t>Color Trend 2016 Duo Lip Color</t>
-  </si>
-  <si>
-    <t>K 07</t>
-  </si>
-  <si>
-    <t>Color Trend 2017 Duo Lip Color</t>
-  </si>
-  <si>
-    <t>Gl 01</t>
-  </si>
-  <si>
-    <t>Gl 06</t>
-  </si>
-  <si>
-    <t>Gl 05</t>
-  </si>
-  <si>
-    <t>Color Trend 2018 Lip Cream</t>
-  </si>
-  <si>
-    <t>J 06</t>
-  </si>
-  <si>
-    <t>J 04</t>
-  </si>
-  <si>
-    <t>J 07</t>
-  </si>
-  <si>
-    <t>J 03</t>
-  </si>
-  <si>
-    <t>J 01</t>
-  </si>
-  <si>
-    <t>J 02</t>
-  </si>
-  <si>
-    <t>J 05</t>
-  </si>
-  <si>
-    <t>Color Trend 2018 Lip Metallic</t>
-  </si>
-  <si>
-    <t>Lip Colour Matte</t>
-  </si>
-  <si>
-    <t>Lip Color Matte</t>
-  </si>
-  <si>
-    <t>05</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>06</t>
-  </si>
-  <si>
-    <t>07</t>
-  </si>
-  <si>
-    <t>Ct 19 Lite Lip Cream</t>
-  </si>
-  <si>
-    <t>Wi 05</t>
-  </si>
-  <si>
-    <t>Trend 2017 Duo Lip Color</t>
-  </si>
-  <si>
-    <t>Gl 03</t>
-  </si>
-  <si>
-    <t>Two Way Cake</t>
-  </si>
-  <si>
-    <t>Dark</t>
-  </si>
-  <si>
-    <t>03 Dark</t>
-  </si>
-  <si>
-    <t>02 Natural</t>
-  </si>
-  <si>
-    <t>Moisturizer</t>
-  </si>
-  <si>
-    <t>Jeruk</t>
-  </si>
-  <si>
-    <t>Leher</t>
-  </si>
-  <si>
-    <t>Color Trend 2020 Lip Cheek</t>
-  </si>
-  <si>
-    <t>S 03 Serene</t>
-  </si>
-  <si>
-    <t>S 02 Freshly</t>
-  </si>
-  <si>
-    <t>S 01 Rosy</t>
-  </si>
-  <si>
-    <t>35 gr</t>
-  </si>
-  <si>
-    <t>Two Way Cake Energizing Aromatic Refill</t>
-  </si>
-  <si>
-    <t>Putih Langsat</t>
-  </si>
-  <si>
-    <t>Alas Bedak Energizing Aromatic</t>
-  </si>
-  <si>
-    <t>Kuning Gading</t>
-  </si>
-  <si>
-    <t>Kuning Langsat</t>
-  </si>
-  <si>
-    <t>Kuning Pengantin</t>
-  </si>
-  <si>
-    <t>Sawo Matang</t>
-  </si>
-  <si>
-    <t>Color Trend 2020 Cheek Palette</t>
-  </si>
-  <si>
-    <t>Pinkish</t>
-  </si>
-  <si>
-    <t>Loose Powder</t>
-  </si>
-  <si>
-    <t>Butiran</t>
-  </si>
-  <si>
-    <t>Creamy Foundation</t>
-  </si>
-  <si>
     <t>Compact Powder Spf 15</t>
   </si>
   <si>
@@ -1168,10 +1195,16 @@
     <t>Color Trend 2015 Eyeliner Pencil</t>
   </si>
   <si>
-    <t>P 02 Hitam</t>
-  </si>
-  <si>
-    <t>P 03 Putih</t>
+    <t>P 02</t>
+  </si>
+  <si>
+    <t>Hitam</t>
+  </si>
+  <si>
+    <t>P 03</t>
+  </si>
+  <si>
+    <t>Putih</t>
   </si>
   <si>
     <t>Color Trend 2020 Eye Makeup Kit</t>
@@ -1225,9 +1258,6 @@
     <t>Duo Eye Make Up</t>
   </si>
   <si>
-    <t>Hitam</t>
-  </si>
-  <si>
     <t>Color Trend 2017 Liquid Eye Shadow</t>
   </si>
   <si>
@@ -1243,16 +1273,10 @@
     <t>Color Trend 2016 Eye Shadow</t>
   </si>
   <si>
-    <t>K 01</t>
-  </si>
-  <si>
     <t>Color Trend 2017 Eye Shadow Kit</t>
   </si>
   <si>
     <t>Color Trend 16 Eyeshadow</t>
-  </si>
-  <si>
-    <t>K 02</t>
   </si>
 </sst>
 </file>
@@ -1584,7 +1608,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B527"/>
+  <dimension ref="A1:B535"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2411,7 +2435,7 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>102</v>
+        <v>26</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -2419,7 +2443,7 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -2483,7 +2507,7 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -2491,7 +2515,7 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -2795,7 +2819,7 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -2811,7 +2835,7 @@
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -3019,7 +3043,7 @@
         <v>178</v>
       </c>
       <c r="B179" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="180" spans="1:2">
@@ -4419,7 +4443,7 @@
         <v>353</v>
       </c>
       <c r="B354" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="355" spans="1:2">
@@ -4459,7 +4483,7 @@
         <v>358</v>
       </c>
       <c r="B359" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="360" spans="1:2">
@@ -4896,66 +4920,66 @@
     </row>
     <row r="414" spans="1:2">
       <c r="A414" t="s">
-        <v>29</v>
+        <v>413</v>
       </c>
       <c r="B414" t="s">
-        <v>29</v>
+        <v>413</v>
       </c>
     </row>
     <row r="415" spans="1:2">
       <c r="A415" t="s">
-        <v>29</v>
+        <v>414</v>
       </c>
       <c r="B415" t="s">
-        <v>29</v>
+        <v>414</v>
       </c>
     </row>
     <row r="416" spans="1:2">
       <c r="A416" t="s">
-        <v>29</v>
+        <v>415</v>
       </c>
       <c r="B416" t="s">
-        <v>29</v>
+        <v>415</v>
       </c>
     </row>
     <row r="417" spans="1:2">
       <c r="A417" t="s">
-        <v>29</v>
+        <v>416</v>
       </c>
       <c r="B417" t="s">
-        <v>29</v>
+        <v>416</v>
       </c>
     </row>
     <row r="418" spans="1:2">
       <c r="A418" t="s">
-        <v>29</v>
+        <v>417</v>
       </c>
       <c r="B418" t="s">
-        <v>29</v>
+        <v>417</v>
       </c>
     </row>
     <row r="419" spans="1:2">
       <c r="A419" t="s">
-        <v>29</v>
+        <v>418</v>
       </c>
       <c r="B419" t="s">
-        <v>29</v>
+        <v>418</v>
       </c>
     </row>
     <row r="420" spans="1:2">
       <c r="A420" t="s">
-        <v>29</v>
+        <v>419</v>
       </c>
       <c r="B420" t="s">
-        <v>29</v>
+        <v>419</v>
       </c>
     </row>
     <row r="421" spans="1:2">
       <c r="A421" t="s">
-        <v>29</v>
+        <v>420</v>
       </c>
       <c r="B421" t="s">
-        <v>29</v>
+        <v>420</v>
       </c>
     </row>
     <row r="422" spans="1:2">
@@ -5803,6 +5827,70 @@
         <v>29</v>
       </c>
       <c r="B527" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="528" spans="1:2">
+      <c r="A528" t="s">
+        <v>29</v>
+      </c>
+      <c r="B528" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="529" spans="1:2">
+      <c r="A529" t="s">
+        <v>29</v>
+      </c>
+      <c r="B529" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="530" spans="1:2">
+      <c r="A530" t="s">
+        <v>29</v>
+      </c>
+      <c r="B530" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="531" spans="1:2">
+      <c r="A531" t="s">
+        <v>29</v>
+      </c>
+      <c r="B531" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="532" spans="1:2">
+      <c r="A532" t="s">
+        <v>29</v>
+      </c>
+      <c r="B532" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="533" spans="1:2">
+      <c r="A533" t="s">
+        <v>29</v>
+      </c>
+      <c r="B533" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="534" spans="1:2">
+      <c r="A534" t="s">
+        <v>29</v>
+      </c>
+      <c r="B534" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="535" spans="1:2">
+      <c r="A535" t="s">
+        <v>29</v>
+      </c>
+      <c r="B535" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>